<commit_message>
has cycle linked list
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adjmnz/Coding/cracking_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC62BA0-D47F-DD42-A154-D2C7926CF683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7AB31-5968-F44B-B7EA-A2BD36C8A964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="520" windowWidth="32420" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="32420" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems Records" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="699">
   <si>
     <t>Problem</t>
   </si>
@@ -2123,6 +2123,12 @@
   </si>
   <si>
     <t>Super interesante. REVISAR</t>
+  </si>
+  <si>
+    <t>Tricky cómo calcular el numerod e subsequencias (2**(r-l))</t>
+  </si>
+  <si>
+    <t>Nice thinking!!!</t>
   </si>
 </sst>
 </file>
@@ -2205,7 +2211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2240,6 +2246,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2461,7 +2468,7 @@
   <dimension ref="A1:AQ929"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="A296" sqref="A296"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2472,7 +2479,7 @@
     <col min="4" max="4" width="15.1640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="33.6640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="14.5" style="4"/>
-    <col min="7" max="7" width="39.1640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="68.6640625" style="4" customWidth="1"/>
     <col min="8" max="8" width="37.83203125" style="4" customWidth="1"/>
     <col min="9" max="23" width="14.5" style="4"/>
     <col min="24" max="24" width="11" style="4" customWidth="1"/>
@@ -3358,23 +3365,23 @@
       </c>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="17" t="str">
+      <c r="A20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>3SUM</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="11" t="s">
+      <c r="B20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="12">
+      <c r="D20" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="8">
         <v>44433</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="9" t="s">
         <v>73</v>
       </c>
       <c r="G20" s="11"/>
@@ -5487,23 +5494,23 @@
       </c>
     </row>
     <row r="90" spans="1:27" ht="16">
-      <c r="A90" s="10" t="str">
+      <c r="A90" s="5" t="str">
         <f t="shared" si="4"/>
         <v>Daily Temperatures</v>
       </c>
-      <c r="B90" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C90" s="11" t="s">
+      <c r="B90" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D90" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="12">
+      <c r="D90" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="8">
         <v>44440</v>
       </c>
-      <c r="F90" s="13" t="s">
+      <c r="F90" s="9" t="s">
         <v>219</v>
       </c>
       <c r="Y90" s="11"/>
@@ -5711,24 +5718,27 @@
       </c>
     </row>
     <row r="98" spans="1:27" ht="16">
-      <c r="A98" s="10" t="str">
+      <c r="A98" s="5" t="str">
         <f t="shared" si="4"/>
         <v>Number of Subsequences with Given Sum</v>
       </c>
-      <c r="B98" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C98" s="11" t="s">
+      <c r="B98" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D98" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="12">
+      <c r="D98" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="8">
         <v>44443</v>
       </c>
-      <c r="F98" s="13" t="s">
+      <c r="F98" s="9" t="s">
         <v>256</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>697</v>
       </c>
       <c r="Y98" s="11"/>
       <c r="Z98" s="14" t="s">
@@ -5902,23 +5912,23 @@
       </c>
     </row>
     <row r="105" spans="1:27" ht="16">
-      <c r="A105" s="10" t="str">
+      <c r="A105" s="5" t="str">
         <f t="shared" si="4"/>
         <v>4SUM</v>
       </c>
-      <c r="B105" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C105" s="11" t="s">
+      <c r="B105" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C105" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D105" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E105" s="12">
+      <c r="D105" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="8">
         <v>44443</v>
       </c>
-      <c r="F105" s="13" t="s">
+      <c r="F105" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Y105" s="11"/>
@@ -6097,24 +6107,27 @@
       </c>
     </row>
     <row r="112" spans="1:27" ht="16">
-      <c r="A112" s="10" t="str">
+      <c r="A112" s="5" t="str">
         <f t="shared" si="4"/>
         <v>Jump Game</v>
       </c>
-      <c r="B112" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C112" s="11" t="s">
+      <c r="B112" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C112" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D112" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="12">
+      <c r="D112" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="8">
         <v>44448</v>
       </c>
-      <c r="F112" s="13" t="s">
+      <c r="F112" s="9" t="s">
         <v>92</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>698</v>
       </c>
       <c r="Y112" s="11"/>
       <c r="Z112" s="14" t="s">
@@ -6289,23 +6302,23 @@
       </c>
     </row>
     <row r="119" spans="1:27" ht="16">
-      <c r="A119" s="10" t="str">
+      <c r="A119" s="5" t="str">
         <f t="shared" si="4"/>
         <v>Group Anagrams</v>
       </c>
-      <c r="B119" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C119" s="11" t="s">
+      <c r="B119" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C119" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D119" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E119" s="12">
+      <c r="D119" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="8">
         <v>44429</v>
       </c>
-      <c r="F119" s="13" t="s">
+      <c r="F119" s="9" t="s">
         <v>69</v>
       </c>
       <c r="Y119" s="11"/>

</xml_diff>

<commit_message>
delete kth from list
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adjmnz/Coding/cracking_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7AB31-5968-F44B-B7EA-A2BD36C8A964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3E16A3-CAAE-EC45-9B1D-8266549903DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="500" windowWidth="32420" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2468,7 +2468,7 @@
   <dimension ref="A1:AQ929"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2747,23 +2747,23 @@
       </c>
     </row>
     <row r="6" spans="1:43" ht="15.75" customHeight="1">
-      <c r="A6" s="10" t="str">
+      <c r="A6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Linked List Cycle</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="D6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
         <v>44429</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -7534,23 +7534,23 @@
       </c>
     </row>
     <row r="167" spans="1:27" ht="16">
-      <c r="A167" s="10" t="str">
+      <c r="A167" s="5" t="str">
         <f t="shared" si="5"/>
         <v>Find First and Last Position of Element in Sorted Array</v>
       </c>
-      <c r="B167" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C167" s="11" t="s">
+      <c r="B167" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C167" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D167" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E167" s="12">
+      <c r="D167" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E167" s="8">
         <v>44427</v>
       </c>
-      <c r="F167" s="13" t="s">
+      <c r="F167" s="9" t="s">
         <v>259</v>
       </c>
       <c r="Y167" s="11"/>
@@ -7562,23 +7562,23 @@
       </c>
     </row>
     <row r="168" spans="1:27" ht="16">
-      <c r="A168" s="10" t="str">
+      <c r="A168" s="5" t="str">
         <f t="shared" si="5"/>
         <v>Find Minimum in Rotated Sorted Array</v>
       </c>
-      <c r="B168" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C168" s="11" t="s">
+      <c r="B168" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C168" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D168" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E168" s="12">
+      <c r="D168" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E168" s="8">
         <v>44454</v>
       </c>
-      <c r="F168" s="13" t="s">
+      <c r="F168" s="9" t="s">
         <v>404</v>
       </c>
       <c r="Y168" s="11"/>
@@ -7590,23 +7590,23 @@
       </c>
     </row>
     <row r="169" spans="1:27" ht="16">
-      <c r="A169" s="10" t="str">
+      <c r="A169" s="5" t="str">
         <f t="shared" si="5"/>
         <v>Search a 2D Matrix</v>
       </c>
-      <c r="B169" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C169" s="11" t="s">
+      <c r="B169" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C169" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D169" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E169" s="12">
+      <c r="D169" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E169" s="8">
         <v>44453</v>
       </c>
-      <c r="F169" s="13" t="s">
+      <c r="F169" s="9" t="s">
         <v>69</v>
       </c>
       <c r="Y169" s="11"/>
@@ -13701,7 +13701,7 @@
       <c r="H929" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:E252" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(E2))), AND(ISNUMBER(E2), LEFT(CELL("format", E2))="D"))</formula1>
     </dataValidation>

</xml_diff>